<commit_message>
update data in FL
</commit_message>
<xml_diff>
--- a/tx/data_raw/tx_covid19_20200620total.xlsx
+++ b/tx/data_raw/tx_covid19_20200620total.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CHS-AAU\Epi\Covid\For Ektron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{51631285-7EED-449F-B16F-0AD03CDBCC1B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA8842C1-2C32-44FE-9020-54B568502D33}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="375">
   <si>
-    <t>COVID-19 Total Cases by County, 3/4/2020 - 06/19/20 at 9:30 AM CST</t>
+    <t>COVID-19 Total Cases by County, 3/4/2020 - 06/20/20 at 9:30 AM CST</t>
   </si>
   <si>
     <t>DISCLAIMER: All data are provisional and are subject to change.</t>
@@ -34,401 +34,401 @@
     <t>Population</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-04</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-05</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-06</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-09</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-10</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-11</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-12</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-13</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-15</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-16</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-17</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-18</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-19</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-20</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-21</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-22</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-23</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-24</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-25</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-26</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-27</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-28</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-29</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-30</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 03-31</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-01</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-02</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-03</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-04</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-05</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-06</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-07</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-08</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-09</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-10</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-11</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-12</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-13</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-14</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-15</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-16</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-17</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-18</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-19</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-20</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-21</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-22</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-23</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-24</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-25</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-26</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-27</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-28</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
-_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-29</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 04-30</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-01</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-02</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-03</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-04</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-05</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-06</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-07</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-08</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-09</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-10</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-11</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-12</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-13</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-14</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-15</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-16</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-17</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-18</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-19</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-20</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-21</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-22</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-23</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-24</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-25</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-26</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-27</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-28</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-29</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-30</t>
   </si>
   <si>
-    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t>Cases_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 05-31</t>
   </si>
   <si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>Cases 06-19</t>
+  </si>
+  <si>
+    <t>Cases 06-20</t>
   </si>
   <si>
     <t>Anderson</t>
@@ -1260,7 +1263,7 @@
     <t>Counties Reporting Cases</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes:_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+    <t xml:space="preserve">Notes:_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 </t>
   </si>
   <si>
@@ -1671,29 +1674,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DC268"/>
+  <dimension ref="A1:DD268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="DC260" sqref="CY260:DC260"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="107" width="12" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" customWidth="1"/>
+    <col min="2" max="108" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:108" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:107" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:108" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:107" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:108" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2015,10 +2016,13 @@
       <c r="DC3" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="DD3" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B4" s="4">
         <v>58199</v>
@@ -2338,10 +2342,13 @@
       <c r="DC4">
         <v>1007</v>
       </c>
+      <c r="DD4">
+        <v>1006</v>
+      </c>
     </row>
-    <row r="5" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B5" s="4">
         <v>22269</v>
@@ -2661,10 +2668,13 @@
       <c r="DC5">
         <v>35</v>
       </c>
+      <c r="DD5">
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B6" s="4">
         <v>90437</v>
@@ -2984,10 +2994,13 @@
       <c r="DC6">
         <v>366</v>
       </c>
+      <c r="DD6">
+        <v>380</v>
+      </c>
     </row>
-    <row r="7" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B7" s="4">
         <v>27699</v>
@@ -3307,10 +3320,13 @@
       <c r="DC7">
         <v>7</v>
       </c>
+      <c r="DD7">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B8" s="4">
         <v>8344</v>
@@ -3630,10 +3646,13 @@
       <c r="DC8">
         <v>3</v>
       </c>
+      <c r="DD8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B9" s="4">
         <v>1948</v>
@@ -3953,10 +3972,13 @@
       <c r="DC9">
         <v>3</v>
       </c>
+      <c r="DD9">
+        <v>3</v>
+      </c>
     </row>
-    <row r="10" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B10" s="4">
         <v>51831</v>
@@ -4276,10 +4298,13 @@
       <c r="DC10">
         <v>62</v>
       </c>
+      <c r="DD10">
+        <v>69</v>
+      </c>
     </row>
-    <row r="11" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B11" s="4">
         <v>30402</v>
@@ -4599,10 +4624,13 @@
       <c r="DC11">
         <v>42</v>
       </c>
+      <c r="DD11">
+        <v>43</v>
+      </c>
     </row>
-    <row r="12" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B12" s="4">
         <v>7692</v>
@@ -4922,10 +4950,13 @@
       <c r="DC12">
         <v>83</v>
       </c>
+      <c r="DD12">
+        <v>83</v>
+      </c>
     </row>
-    <row r="13" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B13" s="4">
         <v>21246</v>
@@ -5245,10 +5276,13 @@
       <c r="DC13">
         <v>13</v>
       </c>
+      <c r="DD13">
+        <v>15</v>
+      </c>
     </row>
-    <row r="14" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B14" s="4">
         <v>86105</v>
@@ -5568,10 +5602,13 @@
       <c r="DC14">
         <v>338</v>
       </c>
+      <c r="DD14">
+        <v>340</v>
+      </c>
     </row>
-    <row r="15" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B15" s="4">
         <v>3624</v>
@@ -5891,10 +5928,13 @@
       <c r="DC15">
         <v>1</v>
       </c>
+      <c r="DD15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B16" s="4">
         <v>34445</v>
@@ -6214,10 +6254,13 @@
       <c r="DC16">
         <v>33</v>
       </c>
+      <c r="DD16">
+        <v>34</v>
+      </c>
     </row>
-    <row r="17" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4">
         <v>353629</v>
@@ -6537,10 +6580,13 @@
       <c r="DC17">
         <v>769</v>
       </c>
+      <c r="DD17">
+        <v>818</v>
+      </c>
     </row>
-    <row r="18" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B18" s="4">
         <v>2093502</v>
@@ -6860,10 +6906,13 @@
       <c r="DC18">
         <v>5550</v>
       </c>
+      <c r="DD18">
+        <v>5962</v>
+      </c>
     </row>
-    <row r="19" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B19" s="4">
         <v>11504</v>
@@ -7183,10 +7232,13 @@
       <c r="DC19">
         <v>14</v>
       </c>
+      <c r="DD19">
+        <v>14</v>
+      </c>
     </row>
-    <row r="20" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B20" s="4">
         <v>685</v>
@@ -7506,10 +7558,13 @@
       <c r="DC20">
         <v>0</v>
       </c>
+      <c r="DD20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21" s="4">
         <v>17765</v>
@@ -7829,10 +7884,13 @@
       <c r="DC21">
         <v>7</v>
       </c>
+      <c r="DD21">
+        <v>7</v>
+      </c>
     </row>
-    <row r="22" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B22" s="4">
         <v>92570</v>
@@ -8152,10 +8210,13 @@
       <c r="DC22">
         <v>394</v>
       </c>
+      <c r="DD22">
+        <v>398</v>
+      </c>
     </row>
-    <row r="23" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B23" s="4">
         <v>375869</v>
@@ -8475,10 +8536,13 @@
       <c r="DC23">
         <v>1609</v>
       </c>
+      <c r="DD23">
+        <v>1669</v>
+      </c>
     </row>
-    <row r="24" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B24" s="4">
         <v>229410</v>
@@ -8798,10 +8862,13 @@
       <c r="DC24">
         <v>1095</v>
       </c>
+      <c r="DD24">
+        <v>1163</v>
+      </c>
     </row>
-    <row r="25" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B25" s="4">
         <v>9133</v>
@@ -9121,10 +9188,13 @@
       <c r="DC25">
         <v>24</v>
       </c>
+      <c r="DD25">
+        <v>24</v>
+      </c>
     </row>
-    <row r="26" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B26" s="4">
         <v>1568</v>
@@ -9444,10 +9514,13 @@
       <c r="DC26">
         <v>1</v>
       </c>
+      <c r="DD26">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B27" s="4">
         <v>7175</v>
@@ -9767,10 +9840,13 @@
       <c r="DC27">
         <v>2</v>
       </c>
+      <c r="DD27">
+        <v>2</v>
+      </c>
     </row>
-    <row r="28" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B28" s="4">
         <v>38923</v>
@@ -10090,10 +10166,13 @@
       <c r="DC28">
         <v>62</v>
       </c>
+      <c r="DD28">
+        <v>62</v>
+      </c>
     </row>
-    <row r="29" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B29" s="4">
         <v>17718</v>
@@ -10413,10 +10492,13 @@
       <c r="DC29">
         <v>53</v>
       </c>
+      <c r="DD29">
+        <v>54</v>
+      </c>
     </row>
-    <row r="30" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B30" s="4">
         <v>48196</v>
@@ -10736,10 +10818,13 @@
       <c r="DC30">
         <v>79</v>
       </c>
+      <c r="DD30">
+        <v>80</v>
+      </c>
     </row>
-    <row r="31" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B31" s="4">
         <v>44284</v>
@@ -11059,10 +11144,13 @@
       <c r="DC31">
         <v>197</v>
       </c>
+      <c r="DD31">
+        <v>208</v>
+      </c>
     </row>
-    <row r="32" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B32" s="4">
         <v>22840</v>
@@ -11382,10 +11470,13 @@
       <c r="DC32">
         <v>52</v>
       </c>
+      <c r="DD32">
+        <v>55</v>
+      </c>
     </row>
-    <row r="33" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B33" s="4">
         <v>13456</v>
@@ -11705,10 +11796,13 @@
       <c r="DC33">
         <v>13</v>
       </c>
+      <c r="DD33">
+        <v>13</v>
+      </c>
     </row>
-    <row r="34" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B34" s="4">
         <v>427881</v>
@@ -12028,10 +12122,13 @@
       <c r="DC34">
         <v>1371</v>
       </c>
+      <c r="DD34">
+        <v>1454</v>
+      </c>
     </row>
-    <row r="35" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B35" s="4">
         <v>13322</v>
@@ -12351,10 +12448,13 @@
       <c r="DC35">
         <v>109</v>
       </c>
+      <c r="DD35">
+        <v>110</v>
+      </c>
     </row>
-    <row r="36" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B36" s="4">
         <v>5799</v>
@@ -12674,10 +12774,13 @@
       <c r="DC36">
         <v>6</v>
       </c>
+      <c r="DD36">
+        <v>6</v>
+      </c>
     </row>
-    <row r="37" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B37" s="4">
         <v>30327</v>
@@ -12997,10 +13100,13 @@
       <c r="DC37">
         <v>36</v>
       </c>
+      <c r="DD37">
+        <v>36</v>
+      </c>
     </row>
-    <row r="38" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B38" s="4">
         <v>7103</v>
@@ -13320,10 +13426,13 @@
       <c r="DC38">
         <v>51</v>
       </c>
+      <c r="DD38">
+        <v>51</v>
+      </c>
     </row>
-    <row r="39" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B39" s="4">
         <v>42320</v>
@@ -13643,10 +13752,13 @@
       <c r="DC39">
         <v>138</v>
       </c>
+      <c r="DD39">
+        <v>149</v>
+      </c>
     </row>
-    <row r="40" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B40" s="4">
         <v>52178</v>
@@ -13966,10 +14078,13 @@
       <c r="DC40">
         <v>67</v>
       </c>
+      <c r="DD40">
+        <v>67</v>
+      </c>
     </row>
-    <row r="41" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B41" s="4">
         <v>7062</v>
@@ -14289,10 +14404,13 @@
       <c r="DC41">
         <v>6</v>
       </c>
+      <c r="DD41">
+        <v>6</v>
+      </c>
     </row>
-    <row r="42" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B42" s="4">
         <v>9787</v>
@@ -14612,10 +14730,13 @@
       <c r="DC42">
         <v>5</v>
       </c>
+      <c r="DD42">
+        <v>5</v>
+      </c>
     </row>
-    <row r="43" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B43" s="4">
         <v>3348</v>
@@ -14935,10 +15056,13 @@
       <c r="DC43">
         <v>1</v>
       </c>
+      <c r="DD43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B44" s="4">
         <v>3215</v>
@@ -15258,10 +15382,13 @@
       <c r="DC44">
         <v>4</v>
       </c>
+      <c r="DD44">
+        <v>4</v>
+      </c>
     </row>
-    <row r="45" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B45" s="4">
         <v>8478</v>
@@ -15581,10 +15708,13 @@
       <c r="DC45">
         <v>3</v>
       </c>
+      <c r="DD45">
+        <v>3</v>
+      </c>
     </row>
-    <row r="46" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B46" s="4">
         <v>1039369</v>
@@ -15904,10 +16034,13 @@
       <c r="DC46">
         <v>2026</v>
       </c>
+      <c r="DD46">
+        <v>2064</v>
+      </c>
     </row>
-    <row r="47" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B47" s="4">
         <v>3210</v>
@@ -16227,10 +16360,13 @@
       <c r="DC47">
         <v>5</v>
       </c>
+      <c r="DD47">
+        <v>5</v>
+      </c>
     </row>
-    <row r="48" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B48" s="4">
         <v>21273</v>
@@ -16550,10 +16686,13 @@
       <c r="DC48">
         <v>46</v>
       </c>
+      <c r="DD48">
+        <v>55</v>
+      </c>
     </row>
-    <row r="49" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B49" s="4">
         <v>147330</v>
@@ -16873,10 +17012,13 @@
       <c r="DC49">
         <v>219</v>
       </c>
+      <c r="DD49">
+        <v>240</v>
+      </c>
     </row>
-    <row r="50" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B50" s="4">
         <v>13075</v>
@@ -17196,10 +17338,13 @@
       <c r="DC50">
         <v>14</v>
       </c>
+      <c r="DD50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="51" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B51" s="4">
         <v>4147</v>
@@ -17519,10 +17664,13 @@
       <c r="DC51">
         <v>1</v>
       </c>
+      <c r="DD51">
+        <v>2</v>
+      </c>
     </row>
-    <row r="52" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B52" s="4">
         <v>39727</v>
@@ -17842,10 +17990,13 @@
       <c r="DC52">
         <v>27</v>
       </c>
+      <c r="DD52">
+        <v>27</v>
+      </c>
     </row>
-    <row r="53" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B53" s="4">
         <v>78317</v>
@@ -18165,10 +18316,13 @@
       <c r="DC53">
         <v>305</v>
       </c>
+      <c r="DD53">
+        <v>305</v>
+      </c>
     </row>
-    <row r="54" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B54" s="4">
         <v>1510</v>
@@ -18488,10 +18642,13 @@
       <c r="DC54">
         <v>4</v>
       </c>
+      <c r="DD54">
+        <v>4</v>
+      </c>
     </row>
-    <row r="55" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B55" s="4">
         <v>6209</v>
@@ -18811,10 +18968,13 @@
       <c r="DC55">
         <v>45</v>
       </c>
+      <c r="DD55">
+        <v>46</v>
+      </c>
     </row>
-    <row r="56" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B56" s="4">
         <v>4040</v>
@@ -19134,10 +19294,13 @@
       <c r="DC56">
         <v>5</v>
       </c>
+      <c r="DD56">
+        <v>5</v>
+      </c>
     </row>
-    <row r="57" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B57" s="4">
         <v>6464</v>
@@ -19457,10 +19620,13 @@
       <c r="DC57">
         <v>8</v>
       </c>
+      <c r="DD57">
+        <v>8</v>
+      </c>
     </row>
-    <row r="58" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B58" s="4">
         <v>2245</v>
@@ -19780,10 +19946,13 @@
       <c r="DC58">
         <v>0</v>
       </c>
+      <c r="DD58">
+        <v>1</v>
+      </c>
     </row>
-    <row r="59" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B59" s="4">
         <v>7237</v>
@@ -20103,10 +20272,13 @@
       <c r="DC59">
         <v>49</v>
       </c>
+      <c r="DD59">
+        <v>49</v>
+      </c>
     </row>
-    <row r="60" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B60" s="4">
         <v>2734111</v>
@@ -20426,10 +20598,13 @@
       <c r="DC60">
         <v>15648</v>
       </c>
+      <c r="DD60">
+        <v>16042</v>
+      </c>
     </row>
-    <row r="61" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B61" s="4">
         <v>13592</v>
@@ -20749,10 +20924,13 @@
       <c r="DC61">
         <v>45</v>
       </c>
+      <c r="DD61">
+        <v>45</v>
+      </c>
     </row>
-    <row r="62" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B62" s="4">
         <v>18143</v>
@@ -21072,10 +21250,13 @@
       <c r="DC62">
         <v>233</v>
       </c>
+      <c r="DD62">
+        <v>233</v>
+      </c>
     </row>
-    <row r="63" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B63" s="4">
         <v>5367</v>
@@ -21395,10 +21576,13 @@
       <c r="DC63">
         <v>4</v>
       </c>
+      <c r="DD63">
+        <v>4</v>
+      </c>
     </row>
-    <row r="64" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B64" s="4">
         <v>897953</v>
@@ -21718,10 +21902,13 @@
       <c r="DC64">
         <v>1980</v>
       </c>
+      <c r="DD64">
+        <v>2054</v>
+      </c>
     </row>
-    <row r="65" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B65" s="4">
         <v>21737</v>
@@ -22041,10 +22228,13 @@
       <c r="DC65">
         <v>35</v>
       </c>
+      <c r="DD65">
+        <v>37</v>
+      </c>
     </row>
-    <row r="66" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B66" s="4">
         <v>2174</v>
@@ -22364,10 +22554,13 @@
       <c r="DC66">
         <v>2</v>
       </c>
+      <c r="DD66">
+        <v>2</v>
+      </c>
     </row>
-    <row r="67" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B67" s="4">
         <v>11743</v>
@@ -22687,10 +22880,13 @@
       <c r="DC67">
         <v>3</v>
       </c>
+      <c r="DD67">
+        <v>3</v>
+      </c>
     </row>
-    <row r="68" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B68" s="4">
         <v>3410</v>
@@ -23010,10 +23206,13 @@
       <c r="DC68">
         <v>27</v>
       </c>
+      <c r="DD68">
+        <v>27</v>
+      </c>
     </row>
-    <row r="69" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B69" s="4">
         <v>11796</v>
@@ -23333,10 +23532,13 @@
       <c r="DC69">
         <v>5</v>
       </c>
+      <c r="DD69">
+        <v>5</v>
+      </c>
     </row>
-    <row r="70" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B70" s="4">
         <v>18205</v>
@@ -23656,10 +23858,13 @@
       <c r="DC70">
         <v>7</v>
       </c>
+      <c r="DD70">
+        <v>7</v>
+      </c>
     </row>
-    <row r="71" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B71" s="4">
         <v>184841</v>
@@ -23979,10 +24184,13 @@
       <c r="DC71">
         <v>300</v>
       </c>
+      <c r="DD71">
+        <v>325</v>
+      </c>
     </row>
-    <row r="72" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B72" s="4">
         <v>1991</v>
@@ -24302,10 +24510,13 @@
       <c r="DC72">
         <v>0</v>
       </c>
+      <c r="DD72">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B73" s="4">
         <v>177721</v>
@@ -24625,10 +24836,13 @@
       <c r="DC73">
         <v>510</v>
       </c>
+      <c r="DD73">
+        <v>510</v>
+      </c>
     </row>
-    <row r="74" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B74" s="4">
         <v>876120</v>
@@ -24948,10 +25162,13 @@
       <c r="DC74">
         <v>4178</v>
       </c>
+      <c r="DD74">
+        <v>4340</v>
+      </c>
     </row>
-    <row r="75" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B75" s="4">
         <v>41526</v>
@@ -25271,10 +25488,13 @@
       <c r="DC75">
         <v>44</v>
       </c>
+      <c r="DD75">
+        <v>44</v>
+      </c>
     </row>
-    <row r="76" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B76" s="4">
         <v>16603</v>
@@ -25594,10 +25814,13 @@
       <c r="DC76">
         <v>22</v>
       </c>
+      <c r="DD76">
+        <v>22</v>
+      </c>
     </row>
-    <row r="77" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B77" s="4">
         <v>34597</v>
@@ -25917,10 +26140,13 @@
       <c r="DC77">
         <v>65</v>
       </c>
+      <c r="DD77">
+        <v>65</v>
+      </c>
     </row>
-    <row r="78" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B78" s="4">
         <v>26086</v>
@@ -26240,10 +26466,13 @@
       <c r="DC78">
         <v>52</v>
       </c>
+      <c r="DD78">
+        <v>58</v>
+      </c>
     </row>
-    <row r="79" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B79" s="4">
         <v>3985</v>
@@ -26563,10 +26792,13 @@
       <c r="DC79">
         <v>2</v>
       </c>
+      <c r="DD79">
+        <v>2</v>
+      </c>
     </row>
-    <row r="80" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B80" s="4">
         <v>5786</v>
@@ -26886,10 +27118,13 @@
       <c r="DC80">
         <v>18</v>
       </c>
+      <c r="DD80">
+        <v>18</v>
+      </c>
     </row>
-    <row r="81" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B81" s="4">
         <v>1240</v>
@@ -27209,10 +27444,13 @@
       <c r="DC81">
         <v>0</v>
       </c>
+      <c r="DD81">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B82" s="4">
         <v>840383</v>
@@ -27532,10 +27770,13 @@
       <c r="DC82">
         <v>2726</v>
       </c>
+      <c r="DD82">
+        <v>2882</v>
+      </c>
     </row>
-    <row r="83" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B83" s="4">
         <v>10924</v>
@@ -27855,10 +28096,13 @@
       <c r="DC83">
         <v>30</v>
       </c>
+      <c r="DD83">
+        <v>31</v>
+      </c>
     </row>
-    <row r="84" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B84" s="4">
         <v>19860</v>
@@ -28178,10 +28422,13 @@
       <c r="DC84">
         <v>18</v>
       </c>
+      <c r="DD84">
+        <v>18</v>
+      </c>
     </row>
-    <row r="85" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B85" s="4">
         <v>20023</v>
@@ -28501,10 +28748,13 @@
       <c r="DC85">
         <v>119</v>
       </c>
+      <c r="DD85">
+        <v>130</v>
+      </c>
     </row>
-    <row r="86" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B86" s="4">
         <v>22121</v>
@@ -28824,10 +29074,13 @@
       <c r="DC86">
         <v>14</v>
       </c>
+      <c r="DD86">
+        <v>14</v>
+      </c>
     </row>
-    <row r="87" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B87" s="4">
         <v>355196</v>
@@ -29147,10 +29400,13 @@
       <c r="DC87">
         <v>1535</v>
       </c>
+      <c r="DD87">
+        <v>1642</v>
+      </c>
     </row>
-    <row r="88" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B88" s="4">
         <v>6784</v>
@@ -29470,10 +29726,13 @@
       <c r="DC88">
         <v>7</v>
       </c>
+      <c r="DD88">
+        <v>7</v>
+      </c>
     </row>
-    <row r="89" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B89" s="4">
         <v>26191</v>
@@ -29793,10 +30052,13 @@
       <c r="DC89">
         <v>16</v>
       </c>
+      <c r="DD89">
+        <v>17</v>
+      </c>
     </row>
-    <row r="90" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B90" s="4">
         <v>1365</v>
@@ -30116,10 +30378,13 @@
       <c r="DC90">
         <v>5</v>
       </c>
+      <c r="DD90">
+        <v>5</v>
+      </c>
     </row>
-    <row r="91" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B91" s="4">
         <v>7717</v>
@@ -30439,10 +30704,13 @@
       <c r="DC91">
         <v>7</v>
       </c>
+      <c r="DD91">
+        <v>7</v>
+      </c>
     </row>
-    <row r="92" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B92" s="4">
         <v>21347</v>
@@ -30762,10 +31030,13 @@
       <c r="DC92">
         <v>203</v>
       </c>
+      <c r="DD92">
+        <v>213</v>
+      </c>
     </row>
-    <row r="93" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B93" s="4">
         <v>24252</v>
@@ -31085,10 +31356,13 @@
       <c r="DC93">
         <v>113</v>
       </c>
+      <c r="DD93">
+        <v>113</v>
+      </c>
     </row>
-    <row r="94" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B94" s="4">
         <v>131710</v>
@@ -31408,10 +31682,13 @@
       <c r="DC94">
         <v>491</v>
       </c>
+      <c r="DD94">
+        <v>491</v>
+      </c>
     </row>
-    <row r="95" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B95" s="4">
         <v>125730</v>
@@ -31731,10 +32008,13 @@
       <c r="DC95">
         <v>304</v>
       </c>
+      <c r="DD95">
+        <v>305</v>
+      </c>
     </row>
-    <row r="96" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B96" s="4">
         <v>28930</v>
@@ -32054,10 +32334,13 @@
       <c r="DC96">
         <v>288</v>
       </c>
+      <c r="DD96">
+        <v>289</v>
+      </c>
     </row>
-    <row r="97" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B97" s="4">
         <v>170266</v>
@@ -32377,10 +32660,13 @@
       <c r="DC97">
         <v>280</v>
       </c>
+      <c r="DD97">
+        <v>311</v>
+      </c>
     </row>
-    <row r="98" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B98" s="4">
         <v>33202</v>
@@ -32700,10 +32986,13 @@
       <c r="DC98">
         <v>122</v>
       </c>
+      <c r="DD98">
+        <v>135</v>
+      </c>
     </row>
-    <row r="99" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B99" s="4">
         <v>3305</v>
@@ -33023,10 +33312,13 @@
       <c r="DC99">
         <v>2</v>
       </c>
+      <c r="DD99">
+        <v>2</v>
+      </c>
     </row>
-    <row r="100" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B100" s="4">
         <v>8220</v>
@@ -33346,10 +33638,13 @@
       <c r="DC100">
         <v>18</v>
       </c>
+      <c r="DD100">
+        <v>18</v>
+      </c>
     </row>
-    <row r="101" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B101" s="4">
         <v>5820</v>
@@ -33669,10 +33964,13 @@
       <c r="DC101">
         <v>23</v>
       </c>
+      <c r="DD101">
+        <v>23</v>
+      </c>
     </row>
-    <row r="102" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B102" s="4">
         <v>3870</v>
@@ -33992,10 +34290,13 @@
       <c r="DC102">
         <v>4</v>
       </c>
+      <c r="DD102">
+        <v>4</v>
+      </c>
     </row>
-    <row r="103" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B103" s="4">
         <v>56486</v>
@@ -34315,10 +34616,13 @@
       <c r="DC103">
         <v>167</v>
       </c>
+      <c r="DD103">
+        <v>172</v>
+      </c>
     </row>
-    <row r="104" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B104" s="4">
         <v>4978845</v>
@@ -34638,10 +34942,13 @@
       <c r="DC104">
         <v>18552</v>
       </c>
+      <c r="DD104">
+        <v>19739</v>
+      </c>
     </row>
-    <row r="105" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B105" s="4">
         <v>68247</v>
@@ -34961,10 +35268,13 @@
       <c r="DC105">
         <v>268</v>
       </c>
+      <c r="DD105">
+        <v>271</v>
+      </c>
     </row>
-    <row r="106" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B106" s="4">
         <v>6067</v>
@@ -35284,10 +35594,13 @@
       <c r="DC106">
         <v>13</v>
       </c>
+      <c r="DD106">
+        <v>13</v>
+      </c>
     </row>
-    <row r="107" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B107" s="4">
         <v>6197</v>
@@ -35607,10 +35920,13 @@
       <c r="DC107">
         <v>4</v>
       </c>
+      <c r="DD107">
+        <v>4</v>
+      </c>
     </row>
-    <row r="108" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B108" s="4">
         <v>234896</v>
@@ -35930,10 +36246,13 @@
       <c r="DC108">
         <v>1448</v>
       </c>
+      <c r="DD108">
+        <v>1551</v>
+      </c>
     </row>
-    <row r="109" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B109" s="4">
         <v>4644</v>
@@ -36253,10 +36572,13 @@
       <c r="DC109">
         <v>2</v>
       </c>
+      <c r="DD109">
+        <v>2</v>
+      </c>
     </row>
-    <row r="110" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B110" s="4">
         <v>81179</v>
@@ -36576,10 +36898,13 @@
       <c r="DC110">
         <v>94</v>
       </c>
+      <c r="DD110">
+        <v>97</v>
+      </c>
     </row>
-    <row r="111" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B111" s="4">
         <v>870366</v>
@@ -36899,10 +37224,13 @@
       <c r="DC111">
         <v>1447</v>
       </c>
+      <c r="DD111">
+        <v>1556</v>
+      </c>
     </row>
-    <row r="112" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B112" s="4">
         <v>35673</v>
@@ -37222,10 +37550,13 @@
       <c r="DC112">
         <v>47</v>
       </c>
+      <c r="DD112">
+        <v>48</v>
+      </c>
     </row>
-    <row r="113" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B113" s="4">
         <v>24636</v>
@@ -37545,10 +37876,13 @@
       <c r="DC113">
         <v>29</v>
       </c>
+      <c r="DD113">
+        <v>29</v>
+      </c>
     </row>
-    <row r="114" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B114" s="4">
         <v>58643</v>
@@ -37868,10 +38202,13 @@
       <c r="DC114">
         <v>35</v>
       </c>
+      <c r="DD114">
+        <v>35</v>
+      </c>
     </row>
-    <row r="115" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B115" s="4">
         <v>37040</v>
@@ -38191,10 +38528,13 @@
       <c r="DC115">
         <v>48</v>
       </c>
+      <c r="DD115">
+        <v>48</v>
+      </c>
     </row>
-    <row r="116" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B116" s="4">
         <v>22620</v>
@@ -38514,10 +38854,13 @@
       <c r="DC116">
         <v>147</v>
       </c>
+      <c r="DD116">
+        <v>148</v>
+      </c>
     </row>
-    <row r="117" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B117" s="4">
         <v>41236</v>
@@ -38837,10 +39180,13 @@
       <c r="DC117">
         <v>24</v>
       </c>
+      <c r="DD117">
+        <v>26</v>
+      </c>
     </row>
-    <row r="118" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B118" s="4">
         <v>3400</v>
@@ -39160,10 +39506,13 @@
       <c r="DC118">
         <v>14</v>
       </c>
+      <c r="DD118">
+        <v>14</v>
+      </c>
     </row>
-    <row r="119" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B119" s="4">
         <v>95324</v>
@@ -39483,10 +39832,13 @@
       <c r="DC119">
         <v>227</v>
       </c>
+      <c r="DD119">
+        <v>246</v>
+      </c>
     </row>
-    <row r="120" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="4">
         <v>21461</v>
@@ -39806,10 +40158,13 @@
       <c r="DC120">
         <v>49</v>
       </c>
+      <c r="DD120">
+        <v>49</v>
+      </c>
     </row>
-    <row r="121" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B121" s="4">
         <v>1508</v>
@@ -40129,10 +40484,13 @@
       <c r="DC121">
         <v>1</v>
       </c>
+      <c r="DD121">
+        <v>1</v>
+      </c>
     </row>
-    <row r="122" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B122" s="4">
         <v>8841</v>
@@ -40452,10 +40810,13 @@
       <c r="DC122">
         <v>4</v>
       </c>
+      <c r="DD122">
+        <v>4</v>
+      </c>
     </row>
-    <row r="123" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B123" s="4">
         <v>15899</v>
@@ -40775,10 +41136,13 @@
       <c r="DC123">
         <v>24</v>
       </c>
+      <c r="DD123">
+        <v>25</v>
+      </c>
     </row>
-    <row r="124" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B124" s="4">
         <v>35525</v>
@@ -41098,10 +41462,13 @@
       <c r="DC124">
         <v>33</v>
       </c>
+      <c r="DD124">
+        <v>35</v>
+      </c>
     </row>
-    <row r="125" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B125" s="4">
         <v>2113</v>
@@ -41421,10 +41788,13 @@
       <c r="DC125">
         <v>0</v>
       </c>
+      <c r="DD125">
+        <v>0</v>
+      </c>
     </row>
-    <row r="126" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B126" s="4">
         <v>258678</v>
@@ -41744,10 +42114,13 @@
       <c r="DC126">
         <v>1356</v>
       </c>
+      <c r="DD126">
+        <v>1388</v>
+      </c>
     </row>
-    <row r="127" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B127" s="4">
         <v>5077</v>
@@ -42067,10 +42440,13 @@
       <c r="DC127">
         <v>6</v>
       </c>
+      <c r="DD127">
+        <v>8</v>
+      </c>
     </row>
-    <row r="128" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B128" s="4">
         <v>42890</v>
@@ -42390,10 +42766,13 @@
       <c r="DC128">
         <v>21</v>
       </c>
+      <c r="DD128">
+        <v>22</v>
+      </c>
     </row>
-    <row r="129" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B129" s="4">
         <v>171701</v>
@@ -42713,10 +43092,13 @@
       <c r="DC129">
         <v>254</v>
       </c>
+      <c r="DD129">
+        <v>254</v>
+      </c>
     </row>
-    <row r="130" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B130" s="4">
         <v>19735</v>
@@ -43036,10 +43418,13 @@
       <c r="DC130">
         <v>610</v>
       </c>
+      <c r="DD130">
+        <v>650</v>
+      </c>
     </row>
-    <row r="131" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B131" s="4">
         <v>15393</v>
@@ -43359,10 +43744,13 @@
       <c r="DC131">
         <v>11</v>
       </c>
+      <c r="DD131">
+        <v>14</v>
+      </c>
     </row>
-    <row r="132" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B132" s="4">
         <v>125134</v>
@@ -43682,10 +44070,13 @@
       <c r="DC132">
         <v>360</v>
       </c>
+      <c r="DD132">
+        <v>360</v>
+      </c>
     </row>
-    <row r="133" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B133" s="4">
         <v>46278</v>
@@ -44005,10 +44396,13 @@
       <c r="DC133">
         <v>44</v>
       </c>
+      <c r="DD133">
+        <v>44</v>
+      </c>
     </row>
-    <row r="134" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B134" s="4">
         <v>476</v>
@@ -44328,10 +44722,13 @@
       <c r="DC134">
         <v>0</v>
       </c>
+      <c r="DD134">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B135" s="4">
         <v>795</v>
@@ -44651,10 +45048,13 @@
       <c r="DC135">
         <v>0</v>
       </c>
+      <c r="DD135">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B136" s="4">
         <v>52267</v>
@@ -44974,10 +45374,13 @@
       <c r="DC136">
         <v>32</v>
       </c>
+      <c r="DD136">
+        <v>33</v>
+      </c>
     </row>
-    <row r="137" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B137" s="4">
         <v>4344</v>
@@ -45297,10 +45700,13 @@
       <c r="DC137">
         <v>1</v>
       </c>
+      <c r="DD137">
+        <v>1</v>
+      </c>
     </row>
-    <row r="138" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B138" s="4">
         <v>309</v>
@@ -45620,10 +46026,13 @@
       <c r="DC138">
         <v>0</v>
       </c>
+      <c r="DD138">
+        <v>0</v>
+      </c>
     </row>
-    <row r="139" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B139" s="4">
         <v>3462</v>
@@ -45943,10 +46352,13 @@
       <c r="DC139">
         <v>1</v>
       </c>
+      <c r="DD139">
+        <v>2</v>
+      </c>
     </row>
-    <row r="140" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B140" s="4">
         <v>30987</v>
@@ -46266,10 +46678,13 @@
       <c r="DC140">
         <v>24</v>
       </c>
+      <c r="DD140">
+        <v>25</v>
+      </c>
     </row>
-    <row r="141" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B141" s="4">
         <v>3937</v>
@@ -46589,10 +47004,13 @@
       <c r="DC141">
         <v>1</v>
       </c>
+      <c r="DD141">
+        <v>1</v>
+      </c>
     </row>
-    <row r="142" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B142" s="4">
         <v>50014</v>
@@ -46912,10 +47330,13 @@
       <c r="DC142">
         <v>199</v>
       </c>
+      <c r="DD142">
+        <v>199</v>
+      </c>
     </row>
-    <row r="143" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B143" s="4">
         <v>12776</v>
@@ -47235,10 +47656,13 @@
       <c r="DC143">
         <v>29</v>
       </c>
+      <c r="DD143">
+        <v>29</v>
+      </c>
     </row>
-    <row r="144" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B144" s="4">
         <v>21037</v>
@@ -47558,10 +47982,13 @@
       <c r="DC144">
         <v>15</v>
       </c>
+      <c r="DD144">
+        <v>16</v>
+      </c>
     </row>
-    <row r="145" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B145" s="4">
         <v>8309</v>
@@ -47881,10 +48308,13 @@
       <c r="DC145">
         <v>7</v>
       </c>
+      <c r="DD145">
+        <v>7</v>
+      </c>
     </row>
-    <row r="146" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B146" s="4">
         <v>20735</v>
@@ -48204,10 +48634,13 @@
       <c r="DC146">
         <v>43</v>
       </c>
+      <c r="DD146">
+        <v>68</v>
+      </c>
     </row>
-    <row r="147" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B147" s="4">
         <v>17595</v>
@@ -48527,10 +48960,13 @@
       <c r="DC147">
         <v>47</v>
       </c>
+      <c r="DD147">
+        <v>48</v>
+      </c>
     </row>
-    <row r="148" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B148" s="4">
         <v>17707</v>
@@ -48850,10 +49286,13 @@
       <c r="DC148">
         <v>13</v>
       </c>
+      <c r="DD148">
+        <v>14</v>
+      </c>
     </row>
-    <row r="149" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B149" s="4">
         <v>85284</v>
@@ -49173,10 +49612,13 @@
       <c r="DC149">
         <v>169</v>
       </c>
+      <c r="DD149">
+        <v>177</v>
+      </c>
     </row>
-    <row r="150" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B150" s="4">
         <v>23544</v>
@@ -49496,10 +49938,13 @@
       <c r="DC150">
         <v>40</v>
       </c>
+      <c r="DD150">
+        <v>41</v>
+      </c>
     </row>
-    <row r="151" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B151" s="4">
         <v>3651</v>
@@ -49819,10 +50264,13 @@
       <c r="DC151">
         <v>9</v>
       </c>
+      <c r="DD151">
+        <v>9</v>
+      </c>
     </row>
-    <row r="152" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B152" s="4">
         <v>12030</v>
@@ -50142,10 +50590,13 @@
       <c r="DC152">
         <v>9</v>
       </c>
+      <c r="DD152">
+        <v>9</v>
+      </c>
     </row>
-    <row r="153" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B153" s="4">
         <v>19452</v>
@@ -50465,10 +50916,13 @@
       <c r="DC153">
         <v>5</v>
       </c>
+      <c r="DD153">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B154" s="4">
         <v>92</v>
@@ -50788,10 +51242,13 @@
       <c r="DC154">
         <v>0</v>
       </c>
+      <c r="DD154">
+        <v>0</v>
+      </c>
     </row>
-    <row r="155" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B155" s="4">
         <v>317210</v>
@@ -51111,10 +51568,13 @@
       <c r="DC155">
         <v>1136</v>
       </c>
+      <c r="DD155">
+        <v>1208</v>
+      </c>
     </row>
-    <row r="156" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B156" s="4">
         <v>5588</v>
@@ -51434,10 +51894,13 @@
       <c r="DC156">
         <v>21</v>
       </c>
+      <c r="DD156">
+        <v>21</v>
+      </c>
     </row>
-    <row r="157" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B157" s="4">
         <v>8660</v>
@@ -51757,10 +52220,13 @@
       <c r="DC157">
         <v>4</v>
       </c>
+      <c r="DD157">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B158" s="4">
         <v>253066</v>
@@ -52080,10 +52546,13 @@
       <c r="DC158">
         <v>245</v>
       </c>
+      <c r="DD158">
+        <v>262</v>
+      </c>
     </row>
-    <row r="159" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B159" s="4">
         <v>783</v>
@@ -52403,10 +52872,13 @@
       <c r="DC159">
         <v>0</v>
       </c>
+      <c r="DD159">
+        <v>0</v>
+      </c>
     </row>
-    <row r="160" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B160" s="4">
         <v>14527</v>
@@ -52726,10 +53198,13 @@
       <c r="DC160">
         <v>25</v>
       </c>
+      <c r="DD160">
+        <v>26</v>
+      </c>
     </row>
-    <row r="161" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B161" s="4">
         <v>10294</v>
@@ -53049,10 +53524,13 @@
       <c r="DC161">
         <v>21</v>
       </c>
+      <c r="DD161">
+        <v>21</v>
+      </c>
     </row>
-    <row r="162" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B162" s="4">
         <v>6044</v>
@@ -53372,10 +53850,13 @@
       <c r="DC162">
         <v>5</v>
       </c>
+      <c r="DD162">
+        <v>6</v>
+      </c>
     </row>
-    <row r="163" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B163" s="4">
         <v>3899</v>
@@ -53695,10 +54176,13 @@
       <c r="DC163">
         <v>33</v>
       </c>
+      <c r="DD163">
+        <v>33</v>
+      </c>
     </row>
-    <row r="164" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B164" s="4">
         <v>37064</v>
@@ -54018,10 +54502,13 @@
       <c r="DC164">
         <v>104</v>
       </c>
+      <c r="DD164">
+        <v>105</v>
+      </c>
     </row>
-    <row r="165" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B165" s="4">
         <v>59938</v>
@@ -54341,10 +54828,13 @@
       <c r="DC165">
         <v>206</v>
       </c>
+      <c r="DD165">
+        <v>214</v>
+      </c>
     </row>
-    <row r="166" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B166" s="4">
         <v>50594</v>
@@ -54664,10 +55154,13 @@
       <c r="DC166">
         <v>244</v>
       </c>
+      <c r="DD166">
+        <v>245</v>
+      </c>
     </row>
-    <row r="167" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B167" s="4">
         <v>2188</v>
@@ -54987,10 +55480,13 @@
       <c r="DC167">
         <v>0</v>
       </c>
+      <c r="DD167">
+        <v>0</v>
+      </c>
     </row>
-    <row r="168" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B168" s="4">
         <v>187364</v>
@@ -55310,10 +55806,13 @@
       <c r="DC168">
         <v>287</v>
       </c>
+      <c r="DD168">
+        <v>322</v>
+      </c>
     </row>
-    <row r="169" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B169" s="4">
         <v>24635</v>
@@ -55633,10 +56132,13 @@
       <c r="DC169">
         <v>56</v>
       </c>
+      <c r="DD169">
+        <v>57</v>
+      </c>
     </row>
-    <row r="170" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B170" s="4">
         <v>4870</v>
@@ -55956,10 +56458,13 @@
       <c r="DC170">
         <v>1</v>
       </c>
+      <c r="DD170">
+        <v>1</v>
+      </c>
     </row>
-    <row r="171" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B171" s="4">
         <v>9865</v>
@@ -56279,10 +56784,13 @@
       <c r="DC171">
         <v>2</v>
       </c>
+      <c r="DD171">
+        <v>2</v>
+      </c>
     </row>
-    <row r="172" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B172" s="4">
         <v>19199</v>
@@ -56602,10 +57110,13 @@
       <c r="DC172">
         <v>12</v>
       </c>
+      <c r="DD172">
+        <v>12</v>
+      </c>
     </row>
-    <row r="173" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B173" s="4">
         <v>613951</v>
@@ -56925,10 +57436,13 @@
       <c r="DC173">
         <v>1484</v>
       </c>
+      <c r="DD173">
+        <v>1555</v>
+      </c>
     </row>
-    <row r="174" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B174" s="4">
         <v>21575</v>
@@ -57248,10 +57762,13 @@
       <c r="DC174">
         <v>877</v>
       </c>
+      <c r="DD174">
+        <v>877</v>
+      </c>
     </row>
-    <row r="175" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B175" s="4">
         <v>12448</v>
@@ -57571,10 +58088,13 @@
       <c r="DC175">
         <v>31</v>
       </c>
+      <c r="DD175">
+        <v>33</v>
+      </c>
     </row>
-    <row r="176" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B176" s="4">
         <v>1172</v>
@@ -57894,10 +58414,13 @@
       <c r="DC176">
         <v>1</v>
       </c>
+      <c r="DD176">
+        <v>1</v>
+      </c>
     </row>
-    <row r="177" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B177" s="4">
         <v>64106</v>
@@ -58217,10 +58740,13 @@
       <c r="DC177">
         <v>341</v>
       </c>
+      <c r="DD177">
+        <v>343</v>
+      </c>
     </row>
-    <row r="178" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B178" s="4">
         <v>47985</v>
@@ -58540,10 +59066,13 @@
       <c r="DC178">
         <v>116</v>
       </c>
+      <c r="DD178">
+        <v>120</v>
+      </c>
     </row>
-    <row r="179" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B179" s="4">
         <v>13724</v>
@@ -58863,10 +59392,13 @@
       <c r="DC179">
         <v>6</v>
       </c>
+      <c r="DD179">
+        <v>6</v>
+      </c>
     </row>
-    <row r="180" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B180" s="4">
         <v>15642</v>
@@ -59186,10 +59718,13 @@
       <c r="DC180">
         <v>8</v>
       </c>
+      <c r="DD180">
+        <v>10</v>
+      </c>
     </row>
-    <row r="181" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B181" s="4">
         <v>383718</v>
@@ -59509,10 +60044,13 @@
       <c r="DC181">
         <v>485</v>
       </c>
+      <c r="DD181">
+        <v>548</v>
+      </c>
     </row>
-    <row r="182" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B182" s="4">
         <v>11309</v>
@@ -59832,10 +60370,13 @@
       <c r="DC182">
         <v>53</v>
       </c>
+      <c r="DD182">
+        <v>53</v>
+      </c>
     </row>
-    <row r="183" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B183" s="4">
         <v>2200</v>
@@ -60155,10 +60696,13 @@
       <c r="DC183">
         <v>4</v>
       </c>
+      <c r="DD183">
+        <v>4</v>
+      </c>
     </row>
-    <row r="184" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B184" s="4">
         <v>86155</v>
@@ -60478,10 +61022,13 @@
       <c r="DC184">
         <v>135</v>
       </c>
+      <c r="DD184">
+        <v>143</v>
+      </c>
     </row>
-    <row r="185" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B185" s="4">
         <v>27859</v>
@@ -60801,10 +61348,13 @@
       <c r="DC185">
         <v>14</v>
       </c>
+      <c r="DD185">
+        <v>14</v>
+      </c>
     </row>
-    <row r="186" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B186" s="4">
         <v>24576</v>
@@ -61124,10 +61674,13 @@
       <c r="DC186">
         <v>191</v>
       </c>
+      <c r="DD186">
+        <v>193</v>
+      </c>
     </row>
-    <row r="187" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B187" s="4">
         <v>135621</v>
@@ -61447,10 +62000,13 @@
       <c r="DC187">
         <v>124</v>
       </c>
+      <c r="DD187">
+        <v>124</v>
+      </c>
     </row>
-    <row r="188" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B188" s="4">
         <v>9200</v>
@@ -61770,10 +62326,13 @@
       <c r="DC188">
         <v>155</v>
       </c>
+      <c r="DD188">
+        <v>155</v>
+      </c>
     </row>
-    <row r="189" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B189" s="4">
         <v>16533</v>
@@ -62093,10 +62652,13 @@
       <c r="DC189">
         <v>112</v>
       </c>
+      <c r="DD189">
+        <v>112</v>
+      </c>
     </row>
-    <row r="190" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B190" s="4">
         <v>49080</v>
@@ -62416,10 +62978,13 @@
       <c r="DC190">
         <v>73</v>
       </c>
+      <c r="DD190">
+        <v>75</v>
+      </c>
     </row>
-    <row r="191" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B191" s="4">
         <v>122706</v>
@@ -62739,10 +63304,13 @@
       <c r="DC191">
         <v>2819</v>
       </c>
+      <c r="DD191">
+        <v>2822</v>
+      </c>
     </row>
-    <row r="192" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B192" s="4">
         <v>5906</v>
@@ -63062,10 +63630,13 @@
       <c r="DC192">
         <v>11</v>
       </c>
+      <c r="DD192">
+        <v>11</v>
+      </c>
     </row>
-    <row r="193" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B193" s="4">
         <v>11378</v>
@@ -63385,10 +63956,13 @@
       <c r="DC193">
         <v>7</v>
       </c>
+      <c r="DD193">
+        <v>8</v>
+      </c>
     </row>
-    <row r="194" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B194" s="4">
         <v>138104</v>
@@ -63708,10 +64282,13 @@
       <c r="DC194">
         <v>771</v>
       </c>
+      <c r="DD194">
+        <v>775</v>
+      </c>
     </row>
-    <row r="195" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B195" s="4">
         <v>4226</v>
@@ -64031,10 +64608,13 @@
       <c r="DC195">
         <v>2</v>
       </c>
+      <c r="DD195">
+        <v>2</v>
+      </c>
     </row>
-    <row r="196" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B196" s="4">
         <v>3407</v>
@@ -64354,10 +64934,13 @@
       <c r="DC196">
         <v>1</v>
       </c>
+      <c r="DD196">
+        <v>1</v>
+      </c>
     </row>
-    <row r="197" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B197" s="4">
         <v>12610</v>
@@ -64677,10 +65260,13 @@
       <c r="DC197">
         <v>96</v>
       </c>
+      <c r="DD197">
+        <v>99</v>
+      </c>
     </row>
-    <row r="198" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B198" s="4">
         <v>15707</v>
@@ -65000,10 +65586,13 @@
       <c r="DC198">
         <v>14</v>
       </c>
+      <c r="DD198">
+        <v>14</v>
+      </c>
     </row>
-    <row r="199" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B199" s="4">
         <v>7573</v>
@@ -65323,10 +65912,13 @@
       <c r="DC199">
         <v>6</v>
       </c>
+      <c r="DD199">
+        <v>6</v>
+      </c>
     </row>
-    <row r="200" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B200" s="4">
         <v>983</v>
@@ -65646,10 +66238,13 @@
       <c r="DC200">
         <v>2</v>
       </c>
+      <c r="DD200">
+        <v>2</v>
+      </c>
     </row>
-    <row r="201" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B201" s="4">
         <v>16888</v>
@@ -65969,10 +66564,13 @@
       <c r="DC201">
         <v>22</v>
       </c>
+      <c r="DD201">
+        <v>23</v>
+      </c>
     </row>
-    <row r="202" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B202" s="4">
         <v>102243</v>
@@ -66292,10 +66890,13 @@
       <c r="DC202">
         <v>228</v>
       </c>
+      <c r="DD202">
+        <v>228</v>
+      </c>
     </row>
-    <row r="203" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B203" s="4">
         <v>11009</v>
@@ -66615,10 +67216,13 @@
       <c r="DC203">
         <v>3</v>
       </c>
+      <c r="DD203">
+        <v>3</v>
+      </c>
     </row>
-    <row r="204" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B204" s="4">
         <v>52767</v>
@@ -66938,10 +67542,13 @@
       <c r="DC204">
         <v>245</v>
       </c>
+      <c r="DD204">
+        <v>250</v>
+      </c>
     </row>
-    <row r="205" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B205" s="4">
         <v>9936</v>
@@ -67261,10 +67868,13 @@
       <c r="DC205">
         <v>15</v>
       </c>
+      <c r="DD205">
+        <v>18</v>
+      </c>
     </row>
-    <row r="206" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B206" s="4">
         <v>8405</v>
@@ -67584,10 +68194,13 @@
       <c r="DC206">
         <v>86</v>
       </c>
+      <c r="DD206">
+        <v>87</v>
+      </c>
     </row>
-    <row r="207" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B207" s="4">
         <v>28844</v>
@@ -67907,10 +68520,13 @@
       <c r="DC207">
         <v>23</v>
       </c>
+      <c r="DD207">
+        <v>23</v>
+      </c>
     </row>
-    <row r="208" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B208" s="4">
         <v>71325</v>
@@ -68230,10 +68846,13 @@
       <c r="DC208">
         <v>66</v>
       </c>
+      <c r="DD208">
+        <v>66</v>
+      </c>
     </row>
-    <row r="209" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B209" s="4">
         <v>5873</v>
@@ -68553,10 +69172,13 @@
       <c r="DC209">
         <v>2</v>
       </c>
+      <c r="DD209">
+        <v>2</v>
+      </c>
     </row>
-    <row r="210" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B210" s="4">
         <v>3312</v>
@@ -68876,10 +69498,13 @@
       <c r="DC210">
         <v>10</v>
       </c>
+      <c r="DD210">
+        <v>12</v>
+      </c>
     </row>
-    <row r="211" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B211" s="4">
         <v>18368</v>
@@ -69199,10 +69824,13 @@
       <c r="DC211">
         <v>29</v>
       </c>
+      <c r="DD211">
+        <v>29</v>
+      </c>
     </row>
-    <row r="212" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B212" s="4">
         <v>3405</v>
@@ -69522,10 +70150,13 @@
       <c r="DC212">
         <v>1</v>
       </c>
+      <c r="DD212">
+        <v>1</v>
+      </c>
     </row>
-    <row r="213" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B213" s="4">
         <v>25545</v>
@@ -69845,10 +70476,13 @@
       <c r="DC213">
         <v>241</v>
       </c>
+      <c r="DD213">
+        <v>253</v>
+      </c>
     </row>
-    <row r="214" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B214" s="4">
         <v>3276</v>
@@ -70168,10 +70802,13 @@
       <c r="DC214">
         <v>30</v>
       </c>
+      <c r="DD214">
+        <v>30</v>
+      </c>
     </row>
-    <row r="215" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B215" s="4">
         <v>235143</v>
@@ -70491,10 +71128,13 @@
       <c r="DC215">
         <v>318</v>
       </c>
+      <c r="DD215">
+        <v>340</v>
+      </c>
     </row>
-    <row r="216" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B216" s="4">
         <v>9294</v>
@@ -70814,10 +71454,13 @@
       <c r="DC216">
         <v>3</v>
       </c>
+      <c r="DD216">
+        <v>3</v>
+      </c>
     </row>
-    <row r="217" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B217" s="4">
         <v>64731</v>
@@ -71137,10 +71780,13 @@
       <c r="DC217">
         <v>203</v>
       </c>
+      <c r="DD217">
+        <v>224</v>
+      </c>
     </row>
-    <row r="218" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B218" s="4">
         <v>9570</v>
@@ -71460,10 +72106,13 @@
       <c r="DC218">
         <v>5</v>
       </c>
+      <c r="DD218">
+        <v>5</v>
+      </c>
     </row>
-    <row r="219" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B219" s="4">
         <v>1252</v>
@@ -71783,10 +72432,13 @@
       <c r="DC219">
         <v>0</v>
       </c>
+      <c r="DD219">
+        <v>0</v>
+      </c>
     </row>
-    <row r="220" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B220" s="4">
         <v>1523</v>
@@ -72106,10 +72758,13 @@
       <c r="DC220">
         <v>0</v>
       </c>
+      <c r="DD220">
+        <v>0</v>
+      </c>
     </row>
-    <row r="221" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B221" s="4">
         <v>4381</v>
@@ -72429,10 +73084,13 @@
       <c r="DC221">
         <v>1</v>
       </c>
+      <c r="DD221">
+        <v>1</v>
+      </c>
     </row>
-    <row r="222" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B222" s="4">
         <v>7414</v>
@@ -72752,10 +73410,13 @@
       <c r="DC222">
         <v>23</v>
       </c>
+      <c r="DD222">
+        <v>23</v>
+      </c>
     </row>
-    <row r="223" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B223" s="4">
         <v>2143755</v>
@@ -73075,10 +73736,13 @@
       <c r="DC223">
         <v>8099</v>
       </c>
+      <c r="DD223">
+        <v>8331</v>
+      </c>
     </row>
-    <row r="224" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B224" s="4">
         <v>139457</v>
@@ -73398,10 +74062,13 @@
       <c r="DC224">
         <v>268</v>
       </c>
+      <c r="DD224">
+        <v>278</v>
+      </c>
     </row>
-    <row r="225" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B225" s="4">
         <v>1054</v>
@@ -73721,10 +74388,13 @@
       <c r="DC225">
         <v>0</v>
       </c>
+      <c r="DD225">
+        <v>0</v>
+      </c>
     </row>
-    <row r="226" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B226" s="4">
         <v>13040</v>
@@ -74044,10 +74714,13 @@
       <c r="DC226">
         <v>14</v>
       </c>
+      <c r="DD226">
+        <v>14</v>
+      </c>
     </row>
-    <row r="227" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B227" s="4">
         <v>1519</v>
@@ -74367,10 +75040,13 @@
       <c r="DC227">
         <v>0</v>
       </c>
+      <c r="DD227">
+        <v>0</v>
+      </c>
     </row>
-    <row r="228" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B228" s="4">
         <v>32953</v>
@@ -74690,10 +75366,13 @@
       <c r="DC228">
         <v>645</v>
       </c>
+      <c r="DD228">
+        <v>652</v>
+      </c>
     </row>
-    <row r="229" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B229" s="4">
         <v>123276</v>
@@ -75013,10 +75692,13 @@
       <c r="DC229">
         <v>171</v>
       </c>
+      <c r="DD229">
+        <v>178</v>
+      </c>
     </row>
-    <row r="230" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B230" s="4">
         <v>1291502</v>
@@ -75336,10 +76018,13 @@
       <c r="DC230">
         <v>4991</v>
       </c>
+      <c r="DD230">
+        <v>5286</v>
+      </c>
     </row>
-    <row r="231" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B231" s="4">
         <v>14233</v>
@@ -75659,10 +76344,13 @@
       <c r="DC231">
         <v>21</v>
       </c>
+      <c r="DD231">
+        <v>22</v>
+      </c>
     </row>
-    <row r="232" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B232" s="4">
         <v>21343</v>
@@ -75982,10 +76670,13 @@
       <c r="DC232">
         <v>14</v>
       </c>
+      <c r="DD232">
+        <v>18</v>
+      </c>
     </row>
-    <row r="233" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B233" s="4">
         <v>41655</v>
@@ -76305,10 +76996,13 @@
       <c r="DC233">
         <v>41</v>
       </c>
+      <c r="DD233">
+        <v>41</v>
+      </c>
     </row>
-    <row r="234" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B234" s="4">
         <v>3983</v>
@@ -76628,10 +77322,13 @@
       <c r="DC234">
         <v>1</v>
       </c>
+      <c r="DD234">
+        <v>1</v>
+      </c>
     </row>
-    <row r="235" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B235" s="4">
         <v>27937</v>
@@ -76951,10 +77648,13 @@
       <c r="DC235">
         <v>31</v>
       </c>
+      <c r="DD235">
+        <v>36</v>
+      </c>
     </row>
-    <row r="236" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B236" s="4">
         <v>48253</v>
@@ -77274,10 +77974,13 @@
       <c r="DC236">
         <v>39</v>
       </c>
+      <c r="DD236">
+        <v>59</v>
+      </c>
     </row>
-    <row r="237" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B237" s="4">
         <v>55469</v>
@@ -77597,10 +78300,13 @@
       <c r="DC237">
         <v>54</v>
       </c>
+      <c r="DD237">
+        <v>54</v>
+      </c>
     </row>
-    <row r="238" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B238" s="4">
         <v>97744</v>
@@ -77920,10 +78626,13 @@
       <c r="DC238">
         <v>241</v>
       </c>
+      <c r="DD238">
+        <v>241</v>
+      </c>
     </row>
-    <row r="239" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B239" s="4">
         <v>73997</v>
@@ -78243,10 +78952,13 @@
       <c r="DC239">
         <v>1890</v>
       </c>
+      <c r="DD239">
+        <v>1905</v>
+      </c>
     </row>
-    <row r="240" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B240" s="4">
         <v>50731</v>
@@ -78566,10 +79278,13 @@
       <c r="DC240">
         <v>104</v>
       </c>
+      <c r="DD240">
+        <v>106</v>
+      </c>
     </row>
-    <row r="241" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B241" s="4">
         <v>13592</v>
@@ -78889,10 +79604,13 @@
       <c r="DC241">
         <v>7</v>
       </c>
+      <c r="DD241">
+        <v>8</v>
+      </c>
     </row>
-    <row r="242" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B242" s="4">
         <v>35155</v>
@@ -79212,10 +79930,13 @@
       <c r="DC242">
         <v>222</v>
       </c>
+      <c r="DD242">
+        <v>224</v>
+      </c>
     </row>
-    <row r="243" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B243" s="4">
         <v>276183</v>
@@ -79535,10 +80256,13 @@
       <c r="DC243">
         <v>854</v>
       </c>
+      <c r="DD243">
+        <v>874</v>
+      </c>
     </row>
-    <row r="244" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B244" s="4">
         <v>41941</v>
@@ -79858,10 +80582,13 @@
       <c r="DC244">
         <v>114</v>
       </c>
+      <c r="DD244">
+        <v>115</v>
+      </c>
     </row>
-    <row r="245" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B245" s="4">
         <v>5783</v>
@@ -80181,10 +80908,13 @@
       <c r="DC245">
         <v>16</v>
       </c>
+      <c r="DD245">
+        <v>16</v>
+      </c>
     </row>
-    <row r="246" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B246" s="4">
         <v>133138</v>
@@ -80504,10 +81234,13 @@
       <c r="DC246">
         <v>150</v>
       </c>
+      <c r="DD246">
+        <v>169</v>
+      </c>
     </row>
-    <row r="247" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B247" s="4">
         <v>13038</v>
@@ -80827,10 +81560,13 @@
       <c r="DC247">
         <v>7</v>
       </c>
+      <c r="DD247">
+        <v>7</v>
+      </c>
     </row>
-    <row r="248" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B248" s="4">
         <v>22134</v>
@@ -81150,10 +81886,13 @@
       <c r="DC248">
         <v>75</v>
       </c>
+      <c r="DD248">
+        <v>82</v>
+      </c>
     </row>
-    <row r="249" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B249" s="4">
         <v>589914</v>
@@ -81473,10 +82212,13 @@
       <c r="DC249">
         <v>1114</v>
       </c>
+      <c r="DD249">
+        <v>1159</v>
+      </c>
     </row>
-    <row r="250" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B250" s="4">
         <v>51802</v>
@@ -81796,10 +82538,13 @@
       <c r="DC250">
         <v>65</v>
       </c>
+      <c r="DD250">
+        <v>69</v>
+      </c>
     </row>
-    <row r="251" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B251" s="4">
         <v>9295</v>
@@ -82119,10 +82864,13 @@
       <c r="DC251">
         <v>6</v>
       </c>
+      <c r="DD251">
+        <v>6</v>
+      </c>
     </row>
-    <row r="252" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B252" s="4">
         <v>65807</v>
@@ -82442,10 +83190,13 @@
       <c r="DC252">
         <v>62</v>
       </c>
+      <c r="DD252">
+        <v>62</v>
+      </c>
     </row>
-    <row r="253" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B253" s="4">
         <v>45292</v>
@@ -82765,10 +83516,13 @@
       <c r="DC253">
         <v>70</v>
       </c>
+      <c r="DD253">
+        <v>71</v>
+      </c>
     </row>
-    <row r="254" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B254" s="4">
         <v>9225</v>
@@ -83088,10 +83842,13 @@
       <c r="DC254">
         <v>11</v>
       </c>
+      <c r="DD254">
+        <v>13</v>
+      </c>
     </row>
-    <row r="255" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B255" s="4">
         <v>18712</v>
@@ -83411,10 +84168,13 @@
       <c r="DC255">
         <v>16</v>
       </c>
+      <c r="DD255">
+        <v>16</v>
+      </c>
     </row>
-    <row r="256" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B256" s="4">
         <v>14409</v>
@@ -83734,10 +84494,13 @@
       <c r="DC256">
         <v>31</v>
       </c>
+      <c r="DD256">
+        <v>32</v>
+      </c>
     </row>
-    <row r="257" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B257" s="4">
         <v>12682</v>
@@ -84057,10 +84820,13 @@
       <c r="DC257">
         <v>13</v>
       </c>
+      <c r="DD257">
+        <v>13</v>
+      </c>
     </row>
-    <row r="258" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B258" s="4">
         <v>29677668</v>
@@ -84380,21 +85146,24 @@
       <c r="DC258">
         <v>103305</v>
       </c>
+      <c r="DD258">
+        <v>107735</v>
+      </c>
     </row>
-    <row r="259" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B259" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="260" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B260" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C260">
         <v>0</v>
@@ -84711,69 +85480,72 @@
       <c r="DC260">
         <v>239</v>
       </c>
+      <c r="DD260">
+        <v>240</v>
+      </c>
     </row>
-    <row r="261" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B261" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="262" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:108" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B262" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="263" spans="1:107" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:108" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A263" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B263" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="264" spans="1:107" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:108" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A264" s="5" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B264" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="265" spans="1:107" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:108" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A265" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B265" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="266" spans="1:107" ht="29" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:108" ht="29" x14ac:dyDescent="0.35">
       <c r="A266" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B266" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="267" spans="1:107" ht="174" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:108" ht="174" x14ac:dyDescent="0.35">
       <c r="A267" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B267" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="268" spans="1:107" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:108" ht="87" x14ac:dyDescent="0.35">
       <c r="A268" s="5" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B268" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>